<commit_message>
improved header functionality and added book viewing to account page
</commit_message>
<xml_diff>
--- a/BookList.xlsx
+++ b/BookList.xlsx
@@ -575,14 +575,10 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
added due date functionality, improvements to user experience
</commit_message>
<xml_diff>
--- a/BookList.xlsx
+++ b/BookList.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,6 +478,11 @@
           <t>Expected Return</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Expected Return.1</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -503,7 +508,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -512,8 +517,9 @@
         </is>
       </c>
       <c r="H2" s="2" t="n">
-        <v>45868</v>
-      </c>
+        <v>45882</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -539,7 +545,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -550,6 +556,7 @@
       <c r="H3" s="2" t="n">
         <v>45875</v>
       </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -575,11 +582,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -605,11 +613,14 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -635,11 +646,14 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="H6" s="2" t="n">
+        <v>45880</v>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -665,11 +679,14 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="H7" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -695,11 +712,18 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>45880</v>
+      </c>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -725,11 +749,18 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>JohnDoe</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>45895</v>
+      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -755,11 +786,14 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="H10" s="2" t="n">
+        <v>45880</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -785,11 +819,14 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="H11" s="2" t="n">
+        <v>45880</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -815,7 +852,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -826,6 +863,7 @@
       <c r="H12" s="2" t="n">
         <v>45878</v>
       </c>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -851,11 +889,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -881,11 +920,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -911,11 +951,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>yes</t>
         </is>
       </c>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
final ui adjustments and touches to staff dashboard
</commit_message>
<xml_diff>
--- a/BookList.xlsx
+++ b/BookList.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -679,12 +679,16 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Galactus</t>
+        </is>
+      </c>
       <c r="H7" s="2" t="n">
-        <v>45881</v>
+        <v>45883</v>
       </c>
       <c r="I7" t="inlineStr"/>
     </row>
@@ -712,14 +716,10 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>no</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>admin</t>
-        </is>
-      </c>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
       <c r="H8" s="2" t="n">
         <v>45880</v>
       </c>
@@ -749,7 +749,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>no</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="H9" s="2" t="n">
-        <v>45895</v>
+        <v>45872</v>
       </c>
       <c r="I9" t="inlineStr"/>
     </row>
@@ -786,12 +786,16 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr"/>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>BillGates</t>
+        </is>
+      </c>
       <c r="H10" s="2" t="n">
-        <v>45880</v>
+        <v>45881</v>
       </c>
       <c r="I10" t="inlineStr"/>
     </row>
@@ -889,11 +893,17 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>admin</t>
+        </is>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>45881</v>
+      </c>
       <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -957,6 +967,805 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>The Night Circus</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Erin Morgenstern</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Fantasy</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>9780385534635</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2011</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Sapiens</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Yuval Noah Harari</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Non-Fiction</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>9780062316097</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2015</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Circe</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Madeline Miller</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Mythology</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>9780316556323</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2018</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Educated</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Tara Westover</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Memoir</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>9780399590504</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2018</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>The Midnight Library</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Matt Haig</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Fantasy</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>9780525559474</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2020</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Pachinko</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Min Jin Lee</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Historical</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>9781455563920</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2017</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>The Martian</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Andy Weir</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Science Fiction</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>9780553418026</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2014</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Galactus</t>
+        </is>
+      </c>
+      <c r="H22" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="I22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>The Alchemist</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Paulo Coelho</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Philosophical</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>9780061122415</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1993</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Normal People</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Sally Rooney</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Drama</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>9781984822178</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2019</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Project Hail Mary</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Andy Weir</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Science Fiction</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>9780593135204</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Bowser</t>
+        </is>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Where the Crawdads Sing</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Delia Owens</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Mystery</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>9780735219106</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2018</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>A Man Called Ove</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Fredrik Backman</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Drama</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>9781476738024</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2012</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr"/>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>The Silent Patient</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Alex Michaelides</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Thriller</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>9781250301697</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2019</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>The Song of Achilles</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Madeline Miller</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Mythology</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>9780062060624</v>
+      </c>
+      <c r="E29" t="n">
+        <v>2012</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Daisy Jones &amp; The Six</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Taylor Jenkins Reid</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Fiction</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>9781524798628</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2019</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr"/>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Klara and the Sun</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Kazuo Ishiguro</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Science Fiction</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>9780593318171</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Mexican Gothic</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Silvia Moreno-Garcia</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Horror</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>9780525620785</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2020</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>JohnDoe</t>
+        </is>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>45856</v>
+      </c>
+      <c r="I32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>The Paris Library</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Janet Skeslien Charles</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Historical</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>9781982134198</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>The Guest List</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Lucy Foley</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Mystery</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>9780062868930</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2020</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>The Seven Husbands of Evelyn Hugo</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Taylor Jenkins Reid</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Drama</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>9781501161933</v>
+      </c>
+      <c r="E35" t="n">
+        <v>2017</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Beach Read</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Emily Henry</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Romance</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>9781984806734</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2020</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>BillGates</t>
+        </is>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>45881</v>
+      </c>
+      <c r="I36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Verity</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Colleen Hoover</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Thriller</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>9781538724736</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2018</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>The Book Thief</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Markus Zusak</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Historical</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>9780375842207</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2005</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Little Fires Everywhere</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Celeste Ng</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Fiction</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>9780735224315</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2017</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>The Paper Palace</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Miranda Cowley Heller</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Fiction</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>9780593329825</v>
+      </c>
+      <c r="E40" t="n">
+        <v>2021</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>